<commit_message>
added objective tab to factor
</commit_message>
<xml_diff>
--- a/BCIS301 – S1 2019 – Gap-Analysis - Jerry Wang, Kieran Abelen, Hanke Zhang.xlsx
+++ b/BCIS301 – S1 2019 – Gap-Analysis - Jerry Wang, Kieran Abelen, Hanke Zhang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\Dropbox\Kieran Third year\BCIS301 _ AMIC700\Assignment 2\BCIS301---AMIC700---Gap-Analysis-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6121CD68-F55C-4EDC-874C-DF02DE157CCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE15A17-DC0A-4B1B-8569-ED440D510F45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>Location</t>
   </si>
@@ -578,6 +578,9 @@
   <si>
     <t>Interview</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Objective</t>
   </si>
 </sst>
 </file>
@@ -714,12 +717,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -761,9 +770,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -814,34 +820,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90C0FEE6-81D6-4E65-BFB3-45C5FD53F6C1}" name="Table13" displayName="Table13" ref="A2:F1048576" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F1048576" xr:uid="{0FA42A31-C09F-4A95-85AB-F5D34F3FE157}"/>
-  <tableColumns count="6">
-    <tableColumn id="9" xr3:uid="{63AAD324-E562-4AAA-A25E-2367846DC04C}" name="Ref" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{5DC8784B-1E25-459B-B274-4C1BC9CC9F5D}" name="Location" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{12AF813D-93D1-4BCA-8955-445901C38269}" name="Summary" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{A5A640DE-D816-49CF-9282-D716539BE5AA}" name="Factor" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A804B3A9-4AB4-4805-999B-FECDC0FB6508}" name="Is this a Gap" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{5B25B68A-8AF8-4DC6-929F-57AE2910C1EC}" name="Meta-Factor" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90C0FEE6-81D6-4E65-BFB3-45C5FD53F6C1}" name="Table13" displayName="Table13" ref="A2:G1048576" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A2:G1048576" xr:uid="{0FA42A31-C09F-4A95-85AB-F5D34F3FE157}"/>
+  <tableColumns count="7">
+    <tableColumn id="9" xr3:uid="{63AAD324-E562-4AAA-A25E-2367846DC04C}" name="Ref" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{5DC8784B-1E25-459B-B274-4C1BC9CC9F5D}" name="Location" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{898AF53C-731A-4429-A427-95B8C88B4C28}" name="Objective" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{12AF813D-93D1-4BCA-8955-445901C38269}" name="Summary" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{A5A640DE-D816-49CF-9282-D716539BE5AA}" name="Factor" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{A804B3A9-4AB4-4805-999B-FECDC0FB6508}" name="Is this a Gap" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{5B25B68A-8AF8-4DC6-929F-57AE2910C1EC}" name="Meta-Factor" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46000187-4DF8-42D1-8E61-1CCD9B4F33A7}" name="Table1" displayName="Table1" ref="A2:G1048576" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46000187-4DF8-42D1-8E61-1CCD9B4F33A7}" name="Table1" displayName="Table1" ref="A2:G1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A2:G1048576" xr:uid="{4564A83B-E795-414E-A15C-CC2E67E7E1BB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G3">
     <sortCondition ref="G2:G3"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="9" xr3:uid="{40CD8F54-5D7D-4314-8086-F0C4E8CE116C}" name="Ref" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{9F9E6DB9-0D32-4F05-BFF0-DB43451BF75C}" name="Source" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{AFF1E055-213C-4064-BD74-3CC6EDC4A75C}" name="Objective/Goal" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B8DD23A4-B58B-4653-AE3F-31948D216593}" name="Current State" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{89EF021C-AA72-430D-89FA-0C2123CED66E}" name="Future State" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{427DC161-A0D9-41D9-A494-C3575733222B}" name="Gap" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{68C072C1-5BCD-4A05-B3ED-01263C1BAD6B}" name="Action Plan" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{40CD8F54-5D7D-4314-8086-F0C4E8CE116C}" name="Ref" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{9F9E6DB9-0D32-4F05-BFF0-DB43451BF75C}" name="Source" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{AFF1E055-213C-4064-BD74-3CC6EDC4A75C}" name="Objective/Goal" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{B8DD23A4-B58B-4653-AE3F-31948D216593}" name="Current State" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{89EF021C-AA72-430D-89FA-0C2123CED66E}" name="Future State" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{427DC161-A0D9-41D9-A494-C3575733222B}" name="Gap" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{68C072C1-5BCD-4A05-B3ED-01263C1BAD6B}" name="Action Plan" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1110,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C2334F-B6B5-4D73-9541-9F59E2BBE368}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -1120,20 +1127,21 @@
   <cols>
     <col min="1" max="1" width="9.28515625" style="10" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="56" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="11" customWidth="1"/>
-    <col min="5" max="6" width="19.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="11" customWidth="1"/>
+    <col min="6" max="7" width="19.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="21">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="21">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1141,434 +1149,475 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="12"/>
       <c r="B3" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:7" ht="45">
       <c r="B4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:7" ht="30">
       <c r="B5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:7" ht="45">
       <c r="B6" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75">
+    <row r="7" spans="1:7" ht="75">
       <c r="B7" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30">
+    <row r="8" spans="1:7" ht="30">
       <c r="B8" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:7" ht="30">
       <c r="B9" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="75">
+    <row r="10" spans="1:7" ht="75">
       <c r="B10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="120">
+    <row r="11" spans="1:7" ht="120">
       <c r="B11" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="135">
+    <row r="12" spans="1:7" ht="135">
       <c r="B12" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="135">
+    <row r="13" spans="1:7" ht="135">
       <c r="B13" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:7" ht="45">
       <c r="B14" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="165">
+    <row r="15" spans="1:7" ht="165">
       <c r="B15" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="255">
+    <row r="16" spans="1:7" ht="255">
       <c r="B16" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="180">
+    <row r="17" spans="2:5" ht="180">
       <c r="B17" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="150">
+    <row r="18" spans="2:5" ht="150">
       <c r="B18" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="180">
+    <row r="19" spans="2:5" ht="180">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="240">
+    <row r="20" spans="2:5" ht="240">
       <c r="B20" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="135">
+    <row r="21" spans="2:5" ht="135">
       <c r="B21" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E21" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="225">
+    <row r="22" spans="2:5" ht="225">
       <c r="B22" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="150">
+    <row r="23" spans="2:5" ht="150">
       <c r="B23" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="180">
+    <row r="24" spans="2:5" ht="180">
       <c r="B24" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="E24" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="105">
+    <row r="25" spans="2:5" ht="105">
       <c r="B25" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="165">
+    <row r="26" spans="2:5" ht="165">
       <c r="B26" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="105">
+    <row r="27" spans="2:5" ht="105">
       <c r="B27" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="14"/>
+      <c r="D27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="180">
+    <row r="28" spans="2:5" ht="180">
       <c r="B28" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="120">
+    <row r="29" spans="2:5" ht="120">
       <c r="B29" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="14"/>
+      <c r="D29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="75">
+    <row r="30" spans="2:5" ht="75">
       <c r="B30" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="14"/>
+      <c r="D30" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="165">
+    <row r="31" spans="2:5" ht="165">
       <c r="B31" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="E31" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="135">
+    <row r="32" spans="2:5" ht="135">
       <c r="B32" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="135">
+    <row r="33" spans="2:5" ht="135">
       <c r="B33" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="14"/>
+      <c r="D33" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="E33" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="90">
+    <row r="34" spans="2:5" ht="90">
       <c r="B34" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="14"/>
+      <c r="D34" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="270">
+    <row r="35" spans="2:5" ht="270">
       <c r="B35" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="90">
+    <row r="36" spans="2:5" ht="90">
       <c r="B36" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="14"/>
+      <c r="D36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="E36" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="165">
+    <row r="37" spans="2:5" ht="165">
       <c r="B37" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="14"/>
+      <c r="D37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="E37" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="240">
+    <row r="38" spans="2:5" ht="240">
       <c r="B38" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="14"/>
+      <c r="D38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="E38" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="255">
+    <row r="39" spans="2:5" ht="255">
       <c r="B39" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="14"/>
+      <c r="D39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="E39" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="105">
+    <row r="40" spans="2:5" ht="105">
       <c r="B40" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="E40" s="14" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1586,7 +1635,7 @@
   <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>